<commit_message>
03 Aug 2022 Selenium Data Driven frame work
</commit_message>
<xml_diff>
--- a/src/test/resources/materials/AutomationDemoSIte.xlsx
+++ b/src/test/resources/materials/AutomationDemoSIte.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>RunMode</t>
   </si>
@@ -394,10 +394,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -738,7 +743,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="12.59765625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.1328125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="14.1328125" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="16.86328125" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
@@ -858,7 +863,7 @@
       <c r="R2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S2" t="s" s="11">
+      <c r="S2" t="s" s="16">
         <v>97</v>
       </c>
     </row>
@@ -917,7 +922,7 @@
       <c r="R3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S3" t="s" s="12">
+      <c r="S3" t="s" s="17">
         <v>97</v>
       </c>
     </row>
@@ -1033,7 +1038,7 @@
       <c r="R5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S5" t="s" s="13">
+      <c r="S5" t="s" s="18">
         <v>97</v>
       </c>
     </row>
@@ -1092,7 +1097,7 @@
       <c r="R6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S6" t="s" s="14">
+      <c r="S6" t="s" s="19">
         <v>97</v>
       </c>
     </row>
@@ -1208,7 +1213,7 @@
       <c r="R8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S8" t="s" s="15">
+      <c r="S8" t="s" s="20">
         <v>97</v>
       </c>
     </row>

</xml_diff>